<commit_message>
Update test file for test.
The test SharedItemsWithVariousDataTypesInTableColumn  checks
cache definition flags and they didn't change, only pivot table part
has changed.
</commit_message>
<xml_diff>
--- a/ClosedXML.Tests/Resource/Other/PivotTableReferenceFiles/VariousDataTypesInTableColumns/output.xlsx
+++ b/ClosedXML.Tests/Resource/Other/PivotTableReferenceFiles/VariousDataTypesInTableColumns/output.xlsx
@@ -418,267 +418,289 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" dataCaption="Values" showError="0" missingCaption="" showMissing="1" useAutoFormatting="1" pageWrap="0" pageOverThenDown="0" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" indent="0" multipleFieldFilters="0">
-  <x:location ref="A3" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <x:pivotFields count="10">
-    <x:pivotField name="Name" axis="axisRow" showAll="0">
-      <x:items count="2">
-        <x:item x="0"/>
-        <x:item t="default"/>
-      </x:items>
-    </x:pivotField>
-    <x:pivotField name="Only blanks" axis="axisRow" showAll="0">
-      <x:items count="2">
-        <x:item x="0"/>
-        <x:item t="default"/>
-      </x:items>
-    </x:pivotField>
-    <x:pivotField name="Numbers with integers" axis="axisRow" showAll="0">
-      <x:items count="4">
-        <x:item x="0"/>
-        <x:item x="1"/>
-        <x:item x="2"/>
-        <x:item t="default"/>
-      </x:items>
-    </x:pivotField>
-    <x:pivotField name="Numers without integers" axis="axisRow" showAll="0">
-      <x:items count="4">
-        <x:item x="0"/>
-        <x:item x="1"/>
-        <x:item x="2"/>
-        <x:item t="default"/>
-      </x:items>
-    </x:pivotField>
-    <x:pivotField name="Text" axis="axisRow" showAll="0">
-      <x:items count="4">
-        <x:item x="0"/>
-        <x:item x="1"/>
-        <x:item x="2"/>
-        <x:item t="default"/>
-      </x:items>
-    </x:pivotField>
-    <x:pivotField name="Text with long text" axis="axisRow" showAll="0">
-      <x:items count="4">
-        <x:item x="0"/>
-        <x:item x="1"/>
-        <x:item x="2"/>
-        <x:item t="default"/>
-      </x:items>
-    </x:pivotField>
-    <x:pivotField name="DateTime" axis="axisCol" showAll="0">
-      <x:items count="6">
-        <x:item x="0"/>
-        <x:item x="1"/>
-        <x:item x="2"/>
-        <x:item x="3"/>
-        <x:item x="4"/>
-        <x:item t="default"/>
-      </x:items>
-    </x:pivotField>
-    <x:pivotField name="DateTime with num" axis="axisCol" showAll="0">
-      <x:items count="8">
-        <x:item x="0"/>
-        <x:item x="1"/>
-        <x:item x="2"/>
-        <x:item x="3"/>
-        <x:item x="4"/>
-        <x:item x="5"/>
-        <x:item x="6"/>
-        <x:item t="default"/>
-      </x:items>
-    </x:pivotField>
-    <x:pivotField name="Errors" axis="axisCol" showAll="0">
-      <x:items count="5">
-        <x:item x="0"/>
-        <x:item x="1"/>
-        <x:item x="2"/>
-        <x:item x="3"/>
-        <x:item t="default"/>
-      </x:items>
-    </x:pivotField>
-    <x:pivotField name="Mixed Types" axis="axisCol" showAll="0">
-      <x:items count="9">
-        <x:item x="0"/>
-        <x:item x="1"/>
-        <x:item x="2"/>
-        <x:item x="3"/>
-        <x:item x="4"/>
-        <x:item x="5"/>
-        <x:item x="6"/>
-        <x:item x="7"/>
-        <x:item t="default"/>
-      </x:items>
-    </x:pivotField>
-  </x:pivotFields>
-  <x:rowFields count="6">
-    <x:field x="0"/>
-    <x:field x="1"/>
-    <x:field x="2"/>
-    <x:field x="3"/>
-    <x:field x="4"/>
-    <x:field x="5"/>
-  </x:rowFields>
-  <x:rowItems count="20">
-    <x:i>
-      <x:x v="0"/>
-    </x:i>
-    <x:i t="grand">
-      <x:x/>
-    </x:i>
-    <x:i>
-      <x:x v="0"/>
-    </x:i>
-    <x:i t="grand">
-      <x:x/>
-    </x:i>
-    <x:i>
-      <x:x v="0"/>
-    </x:i>
-    <x:i>
-      <x:x v="1"/>
-    </x:i>
-    <x:i>
-      <x:x v="2"/>
-    </x:i>
-    <x:i t="grand">
-      <x:x/>
-    </x:i>
-    <x:i>
-      <x:x v="0"/>
-    </x:i>
-    <x:i>
-      <x:x v="1"/>
-    </x:i>
-    <x:i>
-      <x:x v="2"/>
-    </x:i>
-    <x:i t="grand">
-      <x:x/>
-    </x:i>
-    <x:i>
-      <x:x v="0"/>
-    </x:i>
-    <x:i>
-      <x:x v="1"/>
-    </x:i>
-    <x:i>
-      <x:x v="2"/>
-    </x:i>
-    <x:i t="grand">
-      <x:x/>
-    </x:i>
-    <x:i>
-      <x:x v="0"/>
-    </x:i>
-    <x:i>
-      <x:x v="1"/>
-    </x:i>
-    <x:i>
-      <x:x v="2"/>
-    </x:i>
-    <x:i t="grand">
-      <x:x/>
-    </x:i>
-  </x:rowItems>
-  <x:colFields count="4">
-    <x:field x="6"/>
-    <x:field x="7"/>
-    <x:field x="9"/>
-    <x:field x="8"/>
-  </x:colFields>
-  <x:colItems count="28">
-    <x:i>
-      <x:x v="0"/>
-    </x:i>
-    <x:i>
-      <x:x v="1"/>
-    </x:i>
-    <x:i>
-      <x:x v="2"/>
-    </x:i>
-    <x:i>
-      <x:x v="3"/>
-    </x:i>
-    <x:i>
-      <x:x v="4"/>
-    </x:i>
-    <x:i t="grand">
-      <x:x/>
-    </x:i>
-    <x:i>
-      <x:x v="0"/>
-    </x:i>
-    <x:i>
-      <x:x v="1"/>
-    </x:i>
-    <x:i>
-      <x:x v="2"/>
-    </x:i>
-    <x:i>
-      <x:x v="3"/>
-    </x:i>
-    <x:i>
-      <x:x v="4"/>
-    </x:i>
-    <x:i>
-      <x:x v="5"/>
-    </x:i>
-    <x:i>
-      <x:x v="6"/>
-    </x:i>
-    <x:i t="grand">
-      <x:x/>
-    </x:i>
-    <x:i>
-      <x:x v="0"/>
-    </x:i>
-    <x:i>
-      <x:x v="1"/>
-    </x:i>
-    <x:i>
-      <x:x v="2"/>
-    </x:i>
-    <x:i>
-      <x:x v="3"/>
-    </x:i>
-    <x:i t="grand">
-      <x:x/>
-    </x:i>
-    <x:i>
-      <x:x v="0"/>
-    </x:i>
-    <x:i>
-      <x:x v="1"/>
-    </x:i>
-    <x:i>
-      <x:x v="2"/>
-    </x:i>
-    <x:i>
-      <x:x v="3"/>
-    </x:i>
-    <x:i>
-      <x:x v="4"/>
-    </x:i>
-    <x:i>
-      <x:x v="5"/>
-    </x:i>
-    <x:i>
-      <x:x v="6"/>
-    </x:i>
-    <x:i>
-      <x:x v="7"/>
-    </x:i>
-    <x:i t="grand">
-      <x:x/>
-    </x:i>
-  </x:colItems>
-  <x:pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0"/>
-  <x:extLst>
-    <x:ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" enableEdit="0" hideValuesRow="1"/>
-    </x:ext>
-  </x:extLst>
-</x:pivotTableDefinition>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:AG23" firstHeaderRow="1" firstDataRow="5" firstDataCol="1"/>
+  <pivotFields count="10">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="2">
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="2">
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="6">
+        <item x="3"/>
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="4"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="8">
+        <item x="4"/>
+        <item x="5"/>
+        <item x="3"/>
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="6"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="5">
+        <item x="2"/>
+        <item x="1"/>
+        <item x="0"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="9">
+        <item x="3"/>
+        <item x="2"/>
+        <item x="4"/>
+        <item x="1"/>
+        <item x="5"/>
+        <item x="7"/>
+        <item x="6"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="6">
+    <field x="0"/>
+    <field x="1"/>
+    <field x="2"/>
+    <field x="3"/>
+    <field x="4"/>
+    <field x="5"/>
+  </rowFields>
+  <rowItems count="16">
+    <i>
+      <x/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x/>
+    </i>
+    <i r="3">
+      <x/>
+    </i>
+    <i r="4">
+      <x/>
+    </i>
+    <i r="5">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="1"/>
+    </i>
+    <i r="3">
+      <x v="1"/>
+    </i>
+    <i r="4">
+      <x/>
+    </i>
+    <i r="5">
+      <x/>
+    </i>
+    <i r="4">
+      <x v="1"/>
+    </i>
+    <i r="5">
+      <x v="1"/>
+    </i>
+    <i r="2">
+      <x v="2"/>
+    </i>
+    <i r="3">
+      <x v="2"/>
+    </i>
+    <i r="4">
+      <x v="2"/>
+    </i>
+    <i r="5">
+      <x v="2"/>
+    </i>
+  </rowItems>
+  <colFields count="4">
+    <field x="6"/>
+    <field x="7"/>
+    <field x="9"/>
+    <field x="8"/>
+  </colFields>
+  <colItems count="32">
+    <i>
+      <x/>
+      <x v="2"/>
+      <x/>
+      <x v="3"/>
+    </i>
+    <i t="default" r="2">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="1"/>
+      <x/>
+    </i>
+    <i t="default" r="2">
+      <x v="1"/>
+    </i>
+    <i t="default" r="1">
+      <x v="2"/>
+    </i>
+    <i t="default">
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+      <x v="3"/>
+      <x v="7"/>
+      <x v="2"/>
+    </i>
+    <i t="default" r="2">
+      <x v="7"/>
+    </i>
+    <i t="default" r="1">
+      <x v="3"/>
+    </i>
+    <i t="default">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+      <x v="4"/>
+      <x v="3"/>
+      <x v="2"/>
+    </i>
+    <i t="default" r="2">
+      <x v="3"/>
+    </i>
+    <i t="default" r="1">
+      <x v="4"/>
+    </i>
+    <i t="default">
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+      <x v="5"/>
+      <x v="3"/>
+      <x v="1"/>
+    </i>
+    <i t="default" r="2">
+      <x v="3"/>
+    </i>
+    <i t="default" r="1">
+      <x v="5"/>
+    </i>
+    <i t="default">
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+      <x/>
+      <x v="2"/>
+      <x v="3"/>
+    </i>
+    <i t="default" r="2">
+      <x v="2"/>
+    </i>
+    <i t="default" r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+      <x v="2"/>
+      <x v="3"/>
+    </i>
+    <i t="default" r="2">
+      <x v="2"/>
+    </i>
+    <i t="default" r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="6"/>
+      <x v="4"/>
+      <x v="3"/>
+    </i>
+    <i t="default" r="2">
+      <x v="4"/>
+    </i>
+    <i r="2">
+      <x v="5"/>
+      <x v="3"/>
+    </i>
+    <i t="default" r="2">
+      <x v="5"/>
+    </i>
+    <i r="2">
+      <x v="6"/>
+      <x v="3"/>
+    </i>
+    <i t="default" r="2">
+      <x v="6"/>
+    </i>
+    <i t="default" r="1">
+      <x v="6"/>
+    </i>
+    <i t="default">
+      <x v="4"/>
+    </i>
+  </colItems>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition enableEdit="0" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>